<commit_message>
Psych Public and Law Finished
</commit_message>
<xml_diff>
--- a/2017 processed/Forensics PPL.xlsx
+++ b/2017 processed/Forensics PPL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haley\Documents\Psychology\DOOM Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haley\Documents\GitHub\Outliers\2017 processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="141">
   <si>
     <t>Psychology, Public, and Law</t>
   </si>
@@ -263,9 +263,6 @@
     <t>participant error</t>
   </si>
   <si>
-    <t>ANOVA, Tukey’s honest significant difference</t>
-  </si>
-  <si>
     <t>Correlations, one-way ANOVA, multiple regression</t>
   </si>
   <si>
@@ -351,6 +348,106 @@
   </si>
   <si>
     <t>chi squared, descriptives</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Koehler, Schweitzer, Saks, and McQuiston</t>
+  </si>
+  <si>
+    <t>Science, Technology, or the Expert Witness: What Influences Jurors’ Judgments About Forensic Science Testimony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kubiak et al. </t>
+  </si>
+  <si>
+    <t>Do Sexually Victimized Female Prisoners Perceive Justice in Litigation Process and Outcomes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does It Help, Hurt, or Something Else? The Effect of a Something Else Response Alternative on Children’s Performance on Forced-Choice Questions
+</t>
+  </si>
+  <si>
+    <t>London, Hall, and Lytle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA, Chi Squared, </t>
+  </si>
+  <si>
+    <t>Top-Down Processes in Interpersonal Reality Monitoring Assessments</t>
+  </si>
+  <si>
+    <t>Galit Nahari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">participant did not follow instructions </t>
+  </si>
+  <si>
+    <t>Seeing Red: Disgust Reactions to Gruesome Photographs in Color (but not in Black and White) Increase Convictions</t>
+  </si>
+  <si>
+    <t>Jessica Salerno</t>
+  </si>
+  <si>
+    <t>If You Judge, Investigate! Responsibility Reduces Confirmatory Information Processing in Legal Experts</t>
+  </si>
+  <si>
+    <t>Schmittat and Englich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA,  Chi Squared, MANOVA, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">take out </t>
+  </si>
+  <si>
+    <t>participant fell 4 SD above biased assimilation index, 16 experts excluded due to nature of experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA,  Chi Squared, </t>
+  </si>
+  <si>
+    <t>Evaluating Public Perceptions of the Risk Presented by Registered Sex Offenders: Evidence of Crime Control Theater?</t>
+  </si>
+  <si>
+    <t>Kelly M. Socia and Andrew J. Harris</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> without</t>
+  </si>
+  <si>
+    <t>missing data`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descriptive stats, </t>
+  </si>
+  <si>
+    <t>Challenging the Credibility of Alleged Victims of Child Sexual Abuse in Scottish Courts</t>
+  </si>
+  <si>
+    <t>Szojka, Andrews, Lamb, Stolzenberg, and Lyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM-ANOVA, ANOVA, Descriptives, </t>
+  </si>
+  <si>
+    <t>Police Officers’ Ability to Detect Lies Within a Deception Paradigm</t>
+  </si>
+  <si>
+    <t>Wachi et al.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chi Square, ANOVA, </t>
+  </si>
+  <si>
+    <t>Plea Discounts, Time Pressures, and False-Guilty Pleas in Youth and Adults Who Pleaded Guilty to Felonies in New York City</t>
+  </si>
+  <si>
+    <t>Zottoli, Daftary-Kapur, Winters, and Hogan</t>
+  </si>
+  <si>
+    <t>Chi Square, descriptives</t>
   </si>
 </sst>
 </file>
@@ -1112,8 +1209,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A1:AG50" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:AG50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A1:AG49" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:AG49"/>
   <tableColumns count="33">
     <tableColumn id="1" name="Type" dataDxfId="32"/>
     <tableColumn id="2" name="Journal" dataDxfId="31"/>
@@ -1450,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG1091"/>
+  <dimension ref="A1:AG1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C20"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2035,7 +2132,7 @@
         <v>72</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="F10" s="15">
         <v>345</v>
@@ -2084,13 +2181,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="12">
         <v>116</v>
@@ -2129,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="F12" s="12">
         <v>359</v>
@@ -2174,19 +2271,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="12">
         <v>325</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>66</v>
@@ -2198,7 +2295,7 @@
         <v>42</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>78</v>
@@ -2235,10 +2332,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>16</v>
@@ -2259,7 +2356,7 @@
         <v>60</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>78</v>
@@ -2293,13 +2390,13 @@
         <v>0</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>95</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="F15" s="22">
         <v>27098</v>
@@ -2335,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>16</v>
@@ -2364,7 +2461,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
@@ -2381,10 +2478,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>16</v>
@@ -2406,7 +2503,7 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
@@ -2423,13 +2520,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="E18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="12">
         <v>81</v>
@@ -2447,7 +2544,7 @@
         <v>42</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>77</v>
@@ -2486,13 +2583,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="E19" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" s="12">
         <v>28</v>
@@ -2504,13 +2601,13 @@
         <v>66</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>60</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L19" s="12"/>
       <c r="P19" s="4"/>
@@ -2539,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="E20" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="12">
         <v>42</v>
@@ -2576,17 +2673,29 @@
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="12"/>
+      <c r="C21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="15">
+        <v>441</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="11"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="5"/>
@@ -2605,17 +2714,28 @@
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="C22" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="12">
+        <v>315</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="5"/>
@@ -2634,17 +2754,28 @@
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="C23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="12">
+        <v>688</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -2667,17 +2798,28 @@
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="C24" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="12">
+        <v>94</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="5"/>
@@ -2696,17 +2838,28 @@
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="12">
+        <v>120</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="5"/>
@@ -2725,11 +2878,43 @@
       <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D26" s="11"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+    <row r="26" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="12">
+        <v>72</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M26" s="1">
+        <v>71</v>
+      </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="5"/>
@@ -2748,11 +2933,33 @@
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D27" s="11"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+    <row r="27" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="12">
+        <v>193</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="5"/>
@@ -2771,11 +2978,28 @@
       <c r="AF27" s="3"/>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D28" s="11"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+    <row r="28" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="12">
+        <v>381</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -2799,11 +3023,28 @@
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D29" s="11"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+    <row r="29" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="12">
+        <v>90</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="H29" s="11"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -2827,16 +3068,44 @@
       <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D30" s="11"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="11"/>
+    <row r="30" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="12">
+        <v>148</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="L30" s="12"/>
+      <c r="M30" s="12">
+        <v>130</v>
+      </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="5"/>
@@ -2855,17 +3124,46 @@
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D31" s="11"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
+    <row r="31" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1000</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="M31" s="1">
+        <v>915</v>
+      </c>
+      <c r="N31" s="1">
+        <v>85</v>
+      </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="5"/>
@@ -2884,11 +3182,28 @@
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D32" s="11"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+    <row r="32" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="12">
+        <v>66</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="5"/>
@@ -2907,11 +3222,28 @@
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
     </row>
-    <row r="33" spans="3:33" x14ac:dyDescent="0.3">
-      <c r="D33" s="11"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+    <row r="33" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="12">
+        <v>234</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="5"/>
@@ -2930,11 +3262,30 @@
       <c r="AF33" s="3"/>
       <c r="AG33" s="3"/>
     </row>
-    <row r="34" spans="3:33" x14ac:dyDescent="0.3">
-      <c r="D34" s="11"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+    <row r="34" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="12">
+        <v>97</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="5"/>
@@ -2953,15 +3304,11 @@
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
     </row>
-    <row r="35" spans="3:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="D35" s="11"/>
       <c r="E35" s="13"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="12"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="5"/>
@@ -2980,11 +3327,12 @@
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
     </row>
-    <row r="36" spans="3:33" x14ac:dyDescent="0.3">
-      <c r="D36" s="11"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="12"/>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="G36" s="12"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="11"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="5"/>
@@ -3003,31 +3351,31 @@
       <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
     </row>
-    <row r="37" spans="3:33" x14ac:dyDescent="0.3">
-      <c r="G37" s="12"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="11"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
-      <c r="AF37" s="3"/>
-      <c r="AG37" s="3"/>
-    </row>
-    <row r="38" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="8"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="10"/>
+      <c r="AE37" s="10"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+    </row>
+    <row r="38" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -3051,7 +3399,7 @@
       <c r="AF38" s="10"/>
       <c r="AG38" s="10"/>
     </row>
-    <row r="39" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -3075,7 +3423,7 @@
       <c r="AF39" s="10"/>
       <c r="AG39" s="10"/>
     </row>
-    <row r="40" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -3099,7 +3447,7 @@
       <c r="AF40" s="10"/>
       <c r="AG40" s="10"/>
     </row>
-    <row r="41" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -3123,7 +3471,7 @@
       <c r="AF41" s="10"/>
       <c r="AG41" s="10"/>
     </row>
-    <row r="42" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -3147,7 +3495,7 @@
       <c r="AF42" s="10"/>
       <c r="AG42" s="10"/>
     </row>
-    <row r="43" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -3171,7 +3519,7 @@
       <c r="AF43" s="10"/>
       <c r="AG43" s="10"/>
     </row>
-    <row r="44" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -3190,12 +3538,12 @@
       <c r="AA44" s="8"/>
       <c r="AB44" s="7"/>
       <c r="AC44" s="7"/>
-      <c r="AD44" s="10"/>
-      <c r="AE44" s="10"/>
-      <c r="AF44" s="10"/>
-      <c r="AG44" s="10"/>
-    </row>
-    <row r="45" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AD44" s="7"/>
+      <c r="AE44" s="7"/>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+    </row>
+    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -3219,7 +3567,7 @@
       <c r="AF45" s="7"/>
       <c r="AG45" s="7"/>
     </row>
-    <row r="46" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -3243,7 +3591,7 @@
       <c r="AF46" s="7"/>
       <c r="AG46" s="7"/>
     </row>
-    <row r="47" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -3267,7 +3615,7 @@
       <c r="AF47" s="7"/>
       <c r="AG47" s="7"/>
     </row>
-    <row r="48" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -3315,29 +3663,24 @@
       <c r="AF49" s="7"/>
       <c r="AG49" s="7"/>
     </row>
-    <row r="50" spans="3:33" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="8"/>
-      <c r="Y50" s="8"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="8"/>
-      <c r="AB50" s="7"/>
-      <c r="AC50" s="7"/>
-      <c r="AD50" s="7"/>
-      <c r="AE50" s="7"/>
-      <c r="AF50" s="7"/>
-      <c r="AG50" s="7"/>
+    <row r="50" spans="3:33" x14ac:dyDescent="0.3">
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
     </row>
     <row r="51" spans="3:33" x14ac:dyDescent="0.3">
       <c r="P51" s="4"/>
@@ -4018,10 +4361,10 @@
       <c r="AA86" s="5"/>
       <c r="AB86" s="4"/>
       <c r="AC86" s="4"/>
-      <c r="AD86" s="4"/>
-      <c r="AE86" s="4"/>
-      <c r="AF86" s="4"/>
-      <c r="AG86" s="4"/>
+      <c r="AD86" s="3"/>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
     </row>
     <row r="87" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P87" s="4"/>
@@ -5063,9 +5406,9 @@
       <c r="AA141" s="5"/>
       <c r="AB141" s="4"/>
       <c r="AC141" s="4"/>
-      <c r="AD141" s="3"/>
-      <c r="AE141" s="3"/>
-      <c r="AF141" s="3"/>
+      <c r="AD141" s="4"/>
+      <c r="AE141" s="4"/>
+      <c r="AF141" s="4"/>
       <c r="AG141" s="3"/>
     </row>
     <row r="142" spans="16:33" x14ac:dyDescent="0.3">
@@ -5085,7 +5428,7 @@
       <c r="AD142" s="4"/>
       <c r="AE142" s="4"/>
       <c r="AF142" s="4"/>
-      <c r="AG142" s="3"/>
+      <c r="AG142" s="4"/>
     </row>
     <row r="143" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P143" s="4"/>
@@ -5104,7 +5447,7 @@
       <c r="AD143" s="4"/>
       <c r="AE143" s="4"/>
       <c r="AF143" s="4"/>
-      <c r="AG143" s="4"/>
+      <c r="AG143" s="3"/>
     </row>
     <row r="144" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P144" s="4"/>
@@ -5160,7 +5503,7 @@
       <c r="AC146" s="4"/>
       <c r="AD146" s="4"/>
       <c r="AE146" s="4"/>
-      <c r="AF146" s="4"/>
+      <c r="AF146" s="3"/>
       <c r="AG146" s="3"/>
     </row>
     <row r="147" spans="16:33" x14ac:dyDescent="0.3">
@@ -5255,7 +5598,7 @@
       <c r="AC151" s="4"/>
       <c r="AD151" s="4"/>
       <c r="AE151" s="4"/>
-      <c r="AF151" s="3"/>
+      <c r="AF151" s="4"/>
       <c r="AG151" s="3"/>
     </row>
     <row r="152" spans="16:33" x14ac:dyDescent="0.3">
@@ -5291,9 +5634,9 @@
       <c r="AA153" s="5"/>
       <c r="AB153" s="4"/>
       <c r="AC153" s="4"/>
-      <c r="AD153" s="4"/>
-      <c r="AE153" s="4"/>
-      <c r="AF153" s="4"/>
+      <c r="AD153" s="3"/>
+      <c r="AE153" s="3"/>
+      <c r="AF153" s="3"/>
       <c r="AG153" s="3"/>
     </row>
     <row r="154" spans="16:33" x14ac:dyDescent="0.3">
@@ -5709,9 +6052,9 @@
       <c r="AA175" s="5"/>
       <c r="AB175" s="4"/>
       <c r="AC175" s="4"/>
-      <c r="AD175" s="3"/>
-      <c r="AE175" s="3"/>
-      <c r="AF175" s="3"/>
+      <c r="AD175" s="4"/>
+      <c r="AE175" s="4"/>
+      <c r="AF175" s="4"/>
       <c r="AG175" s="3"/>
     </row>
     <row r="176" spans="16:33" x14ac:dyDescent="0.3">
@@ -5748,8 +6091,8 @@
       <c r="AB177" s="4"/>
       <c r="AC177" s="4"/>
       <c r="AD177" s="4"/>
-      <c r="AE177" s="4"/>
-      <c r="AF177" s="4"/>
+      <c r="AE177" s="3"/>
+      <c r="AF177" s="3"/>
       <c r="AG177" s="3"/>
     </row>
     <row r="178" spans="16:33" x14ac:dyDescent="0.3">
@@ -5766,7 +6109,7 @@
       <c r="AA178" s="5"/>
       <c r="AB178" s="4"/>
       <c r="AC178" s="4"/>
-      <c r="AD178" s="4"/>
+      <c r="AD178" s="3"/>
       <c r="AE178" s="3"/>
       <c r="AF178" s="3"/>
       <c r="AG178" s="3"/>
@@ -6298,10 +6641,10 @@
       <c r="AA206" s="5"/>
       <c r="AB206" s="4"/>
       <c r="AC206" s="4"/>
-      <c r="AD206" s="3"/>
-      <c r="AE206" s="3"/>
-      <c r="AF206" s="3"/>
-      <c r="AG206" s="3"/>
+      <c r="AD206" s="4"/>
+      <c r="AE206" s="4"/>
+      <c r="AF206" s="4"/>
+      <c r="AG206" s="4"/>
     </row>
     <row r="207" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P207" s="4"/>
@@ -6472,7 +6815,7 @@
       <c r="AD215" s="4"/>
       <c r="AE215" s="4"/>
       <c r="AF215" s="4"/>
-      <c r="AG215" s="4"/>
+      <c r="AG215" s="3"/>
     </row>
     <row r="216" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P216" s="4"/>
@@ -6488,9 +6831,9 @@
       <c r="AA216" s="5"/>
       <c r="AB216" s="4"/>
       <c r="AC216" s="4"/>
-      <c r="AD216" s="4"/>
-      <c r="AE216" s="4"/>
-      <c r="AF216" s="4"/>
+      <c r="AD216" s="3"/>
+      <c r="AE216" s="3"/>
+      <c r="AF216" s="3"/>
       <c r="AG216" s="3"/>
     </row>
     <row r="217" spans="16:33" x14ac:dyDescent="0.3">
@@ -6811,10 +7154,10 @@
       <c r="AA233" s="5"/>
       <c r="AB233" s="4"/>
       <c r="AC233" s="4"/>
-      <c r="AD233" s="3"/>
-      <c r="AE233" s="3"/>
-      <c r="AF233" s="3"/>
-      <c r="AG233" s="3"/>
+      <c r="AD233" s="4"/>
+      <c r="AE233" s="4"/>
+      <c r="AF233" s="4"/>
+      <c r="AG233" s="4"/>
     </row>
     <row r="234" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P234" s="4"/>
@@ -7229,10 +7572,10 @@
       <c r="AA255" s="5"/>
       <c r="AB255" s="4"/>
       <c r="AC255" s="4"/>
-      <c r="AD255" s="4"/>
-      <c r="AE255" s="4"/>
-      <c r="AF255" s="4"/>
-      <c r="AG255" s="4"/>
+      <c r="AD255" s="3"/>
+      <c r="AE255" s="3"/>
+      <c r="AF255" s="3"/>
+      <c r="AG255" s="3"/>
     </row>
     <row r="256" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P256" s="4"/>
@@ -8103,10 +8446,10 @@
       <c r="AA301" s="5"/>
       <c r="AB301" s="4"/>
       <c r="AC301" s="4"/>
-      <c r="AD301" s="3"/>
-      <c r="AE301" s="3"/>
-      <c r="AF301" s="3"/>
-      <c r="AG301" s="3"/>
+      <c r="AD301" s="4"/>
+      <c r="AE301" s="4"/>
+      <c r="AF301" s="4"/>
+      <c r="AG301" s="4"/>
     </row>
     <row r="302" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P302" s="4"/>
@@ -8122,10 +8465,10 @@
       <c r="AA302" s="5"/>
       <c r="AB302" s="4"/>
       <c r="AC302" s="4"/>
-      <c r="AD302" s="4"/>
-      <c r="AE302" s="4"/>
-      <c r="AF302" s="4"/>
-      <c r="AG302" s="4"/>
+      <c r="AD302" s="3"/>
+      <c r="AE302" s="3"/>
+      <c r="AF302" s="3"/>
+      <c r="AG302" s="3"/>
     </row>
     <row r="303" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P303" s="4"/>
@@ -8654,10 +8997,10 @@
       <c r="AA330" s="5"/>
       <c r="AB330" s="4"/>
       <c r="AC330" s="4"/>
-      <c r="AD330" s="3"/>
-      <c r="AE330" s="3"/>
-      <c r="AF330" s="3"/>
-      <c r="AG330" s="3"/>
+      <c r="AD330" s="4"/>
+      <c r="AE330" s="4"/>
+      <c r="AF330" s="4"/>
+      <c r="AG330" s="4"/>
     </row>
     <row r="331" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P331" s="4"/>
@@ -8676,7 +9019,7 @@
       <c r="AD331" s="4"/>
       <c r="AE331" s="4"/>
       <c r="AF331" s="4"/>
-      <c r="AG331" s="4"/>
+      <c r="AG331" s="3"/>
     </row>
     <row r="332" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P332" s="4"/>
@@ -8714,7 +9057,7 @@
       <c r="AD333" s="4"/>
       <c r="AE333" s="4"/>
       <c r="AF333" s="4"/>
-      <c r="AG333" s="3"/>
+      <c r="AG333" s="4"/>
     </row>
     <row r="334" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P334" s="4"/>
@@ -8768,10 +9111,10 @@
       <c r="AA336" s="5"/>
       <c r="AB336" s="4"/>
       <c r="AC336" s="4"/>
-      <c r="AD336" s="4"/>
-      <c r="AE336" s="4"/>
-      <c r="AF336" s="4"/>
-      <c r="AG336" s="4"/>
+      <c r="AD336" s="3"/>
+      <c r="AE336" s="3"/>
+      <c r="AF336" s="3"/>
+      <c r="AG336" s="3"/>
     </row>
     <row r="337" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P337" s="4"/>
@@ -9129,10 +9472,10 @@
       <c r="AA355" s="5"/>
       <c r="AB355" s="4"/>
       <c r="AC355" s="4"/>
-      <c r="AD355" s="3"/>
-      <c r="AE355" s="3"/>
-      <c r="AF355" s="3"/>
-      <c r="AG355" s="3"/>
+      <c r="AD355" s="4"/>
+      <c r="AE355" s="4"/>
+      <c r="AF355" s="4"/>
+      <c r="AG355" s="4"/>
     </row>
     <row r="356" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P356" s="4"/>
@@ -9189,7 +9532,7 @@
       <c r="AD358" s="4"/>
       <c r="AE358" s="4"/>
       <c r="AF358" s="4"/>
-      <c r="AG358" s="4"/>
+      <c r="AG358" s="3"/>
     </row>
     <row r="359" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P359" s="4"/>
@@ -9205,9 +9548,9 @@
       <c r="AA359" s="5"/>
       <c r="AB359" s="4"/>
       <c r="AC359" s="4"/>
-      <c r="AD359" s="4"/>
-      <c r="AE359" s="4"/>
-      <c r="AF359" s="4"/>
+      <c r="AD359" s="3"/>
+      <c r="AE359" s="3"/>
+      <c r="AF359" s="3"/>
       <c r="AG359" s="3"/>
     </row>
     <row r="360" spans="16:33" x14ac:dyDescent="0.3">
@@ -9699,7 +10042,7 @@
       <c r="AA385" s="5"/>
       <c r="AB385" s="4"/>
       <c r="AC385" s="4"/>
-      <c r="AD385" s="3"/>
+      <c r="AD385" s="4"/>
       <c r="AE385" s="3"/>
       <c r="AF385" s="3"/>
       <c r="AG385" s="3"/>
@@ -9756,7 +10099,7 @@
       <c r="AA388" s="5"/>
       <c r="AB388" s="4"/>
       <c r="AC388" s="4"/>
-      <c r="AD388" s="4"/>
+      <c r="AD388" s="3"/>
       <c r="AE388" s="3"/>
       <c r="AF388" s="3"/>
       <c r="AG388" s="3"/>
@@ -10174,10 +10517,10 @@
       <c r="AA410" s="5"/>
       <c r="AB410" s="4"/>
       <c r="AC410" s="4"/>
-      <c r="AD410" s="3"/>
-      <c r="AE410" s="3"/>
-      <c r="AF410" s="3"/>
-      <c r="AG410" s="3"/>
+      <c r="AD410" s="4"/>
+      <c r="AE410" s="4"/>
+      <c r="AF410" s="4"/>
+      <c r="AG410" s="4"/>
     </row>
     <row r="411" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P411" s="4"/>
@@ -10291,7 +10634,7 @@
       <c r="AD416" s="4"/>
       <c r="AE416" s="4"/>
       <c r="AF416" s="4"/>
-      <c r="AG416" s="4"/>
+      <c r="AG416" s="3"/>
     </row>
     <row r="417" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P417" s="4"/>
@@ -10307,9 +10650,9 @@
       <c r="AA417" s="5"/>
       <c r="AB417" s="4"/>
       <c r="AC417" s="4"/>
-      <c r="AD417" s="4"/>
-      <c r="AE417" s="4"/>
-      <c r="AF417" s="4"/>
+      <c r="AD417" s="3"/>
+      <c r="AE417" s="3"/>
+      <c r="AF417" s="3"/>
       <c r="AG417" s="3"/>
     </row>
     <row r="418" spans="16:33" x14ac:dyDescent="0.3">
@@ -10744,10 +11087,10 @@
       <c r="AA440" s="5"/>
       <c r="AB440" s="4"/>
       <c r="AC440" s="4"/>
-      <c r="AD440" s="3"/>
-      <c r="AE440" s="3"/>
-      <c r="AF440" s="3"/>
-      <c r="AG440" s="3"/>
+      <c r="AD440" s="4"/>
+      <c r="AE440" s="4"/>
+      <c r="AF440" s="4"/>
+      <c r="AG440" s="4"/>
     </row>
     <row r="441" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P441" s="4"/>
@@ -11029,10 +11372,10 @@
       <c r="AA455" s="5"/>
       <c r="AB455" s="4"/>
       <c r="AC455" s="4"/>
-      <c r="AD455" s="4"/>
-      <c r="AE455" s="4"/>
-      <c r="AF455" s="4"/>
-      <c r="AG455" s="4"/>
+      <c r="AD455" s="3"/>
+      <c r="AE455" s="3"/>
+      <c r="AF455" s="3"/>
+      <c r="AG455" s="3"/>
     </row>
     <row r="456" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P456" s="4"/>
@@ -11599,9 +11942,9 @@
       <c r="AA485" s="5"/>
       <c r="AB485" s="4"/>
       <c r="AC485" s="4"/>
-      <c r="AD485" s="3"/>
-      <c r="AE485" s="3"/>
-      <c r="AF485" s="3"/>
+      <c r="AD485" s="4"/>
+      <c r="AE485" s="4"/>
+      <c r="AF485" s="4"/>
       <c r="AG485" s="3"/>
     </row>
     <row r="486" spans="16:33" x14ac:dyDescent="0.3">
@@ -11751,9 +12094,9 @@
       <c r="AA493" s="5"/>
       <c r="AB493" s="4"/>
       <c r="AC493" s="4"/>
-      <c r="AD493" s="4"/>
-      <c r="AE493" s="4"/>
-      <c r="AF493" s="4"/>
+      <c r="AD493" s="3"/>
+      <c r="AE493" s="3"/>
+      <c r="AF493" s="3"/>
       <c r="AG493" s="3"/>
     </row>
     <row r="494" spans="16:33" x14ac:dyDescent="0.3">
@@ -12720,10 +13063,10 @@
       <c r="AA544" s="5"/>
       <c r="AB544" s="4"/>
       <c r="AC544" s="4"/>
-      <c r="AD544" s="3"/>
-      <c r="AE544" s="3"/>
-      <c r="AF544" s="3"/>
-      <c r="AG544" s="3"/>
+      <c r="AD544" s="4"/>
+      <c r="AE544" s="4"/>
+      <c r="AF544" s="4"/>
+      <c r="AG544" s="4"/>
     </row>
     <row r="545" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P545" s="4"/>
@@ -12856,7 +13199,7 @@
       <c r="AD551" s="4"/>
       <c r="AE551" s="4"/>
       <c r="AF551" s="4"/>
-      <c r="AG551" s="4"/>
+      <c r="AG551" s="3"/>
     </row>
     <row r="552" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P552" s="4"/>
@@ -12929,9 +13272,9 @@
       <c r="AA555" s="5"/>
       <c r="AB555" s="4"/>
       <c r="AC555" s="4"/>
-      <c r="AD555" s="4"/>
-      <c r="AE555" s="4"/>
-      <c r="AF555" s="4"/>
+      <c r="AD555" s="3"/>
+      <c r="AE555" s="3"/>
+      <c r="AF555" s="3"/>
       <c r="AG555" s="3"/>
     </row>
     <row r="556" spans="16:33" x14ac:dyDescent="0.3">
@@ -14715,10 +15058,10 @@
       <c r="AA649" s="5"/>
       <c r="AB649" s="4"/>
       <c r="AC649" s="4"/>
-      <c r="AD649" s="3"/>
-      <c r="AE649" s="3"/>
-      <c r="AF649" s="3"/>
-      <c r="AG649" s="3"/>
+      <c r="AD649" s="4"/>
+      <c r="AE649" s="4"/>
+      <c r="AF649" s="4"/>
+      <c r="AG649" s="4"/>
     </row>
     <row r="650" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P650" s="4"/>
@@ -14737,7 +15080,7 @@
       <c r="AD650" s="4"/>
       <c r="AE650" s="4"/>
       <c r="AF650" s="4"/>
-      <c r="AG650" s="4"/>
+      <c r="AG650" s="3"/>
     </row>
     <row r="651" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P651" s="4"/>
@@ -14772,9 +15115,9 @@
       <c r="AA652" s="5"/>
       <c r="AB652" s="4"/>
       <c r="AC652" s="4"/>
-      <c r="AD652" s="4"/>
-      <c r="AE652" s="4"/>
-      <c r="AF652" s="4"/>
+      <c r="AD652" s="3"/>
+      <c r="AE652" s="3"/>
+      <c r="AF652" s="3"/>
       <c r="AG652" s="3"/>
     </row>
     <row r="653" spans="16:33" x14ac:dyDescent="0.3">
@@ -15342,10 +15685,10 @@
       <c r="AA682" s="5"/>
       <c r="AB682" s="4"/>
       <c r="AC682" s="4"/>
-      <c r="AD682" s="3"/>
-      <c r="AE682" s="3"/>
-      <c r="AF682" s="3"/>
-      <c r="AG682" s="3"/>
+      <c r="AD682" s="4"/>
+      <c r="AE682" s="4"/>
+      <c r="AF682" s="4"/>
+      <c r="AG682" s="4"/>
     </row>
     <row r="683" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P683" s="4"/>
@@ -15494,10 +15837,10 @@
       <c r="AA690" s="5"/>
       <c r="AB690" s="4"/>
       <c r="AC690" s="4"/>
-      <c r="AD690" s="4"/>
-      <c r="AE690" s="4"/>
-      <c r="AF690" s="4"/>
-      <c r="AG690" s="4"/>
+      <c r="AD690" s="3"/>
+      <c r="AE690" s="3"/>
+      <c r="AF690" s="3"/>
+      <c r="AG690" s="3"/>
     </row>
     <row r="691" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P691" s="4"/>
@@ -15817,10 +16160,10 @@
       <c r="AA707" s="5"/>
       <c r="AB707" s="4"/>
       <c r="AC707" s="4"/>
-      <c r="AD707" s="3"/>
-      <c r="AE707" s="3"/>
-      <c r="AF707" s="3"/>
-      <c r="AG707" s="3"/>
+      <c r="AD707" s="4"/>
+      <c r="AE707" s="4"/>
+      <c r="AF707" s="4"/>
+      <c r="AG707" s="4"/>
     </row>
     <row r="708" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P708" s="4"/>
@@ -15836,10 +16179,10 @@
       <c r="AA708" s="5"/>
       <c r="AB708" s="4"/>
       <c r="AC708" s="4"/>
-      <c r="AD708" s="4"/>
-      <c r="AE708" s="4"/>
-      <c r="AF708" s="4"/>
-      <c r="AG708" s="4"/>
+      <c r="AD708" s="3"/>
+      <c r="AE708" s="3"/>
+      <c r="AF708" s="3"/>
+      <c r="AG708" s="3"/>
     </row>
     <row r="709" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P709" s="4"/>
@@ -16387,10 +16730,10 @@
       <c r="AA737" s="5"/>
       <c r="AB737" s="4"/>
       <c r="AC737" s="4"/>
-      <c r="AD737" s="3"/>
-      <c r="AE737" s="3"/>
-      <c r="AF737" s="3"/>
-      <c r="AG737" s="3"/>
+      <c r="AD737" s="4"/>
+      <c r="AE737" s="4"/>
+      <c r="AF737" s="4"/>
+      <c r="AG737" s="4"/>
     </row>
     <row r="738" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P738" s="4"/>
@@ -16409,7 +16752,7 @@
       <c r="AD738" s="4"/>
       <c r="AE738" s="4"/>
       <c r="AF738" s="4"/>
-      <c r="AG738" s="4"/>
+      <c r="AG738" s="3"/>
     </row>
     <row r="739" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P739" s="4"/>
@@ -16501,9 +16844,9 @@
       <c r="AA743" s="5"/>
       <c r="AB743" s="4"/>
       <c r="AC743" s="4"/>
-      <c r="AD743" s="4"/>
-      <c r="AE743" s="4"/>
-      <c r="AF743" s="4"/>
+      <c r="AD743" s="3"/>
+      <c r="AE743" s="3"/>
+      <c r="AF743" s="3"/>
       <c r="AG743" s="3"/>
     </row>
     <row r="744" spans="16:33" x14ac:dyDescent="0.3">
@@ -16862,7 +17205,7 @@
       <c r="AA762" s="5"/>
       <c r="AB762" s="4"/>
       <c r="AC762" s="4"/>
-      <c r="AD762" s="3"/>
+      <c r="AD762" s="4"/>
       <c r="AE762" s="3"/>
       <c r="AF762" s="3"/>
       <c r="AG762" s="3"/>
@@ -16920,8 +17263,8 @@
       <c r="AB765" s="4"/>
       <c r="AC765" s="4"/>
       <c r="AD765" s="4"/>
-      <c r="AE765" s="3"/>
-      <c r="AF765" s="3"/>
+      <c r="AE765" s="4"/>
+      <c r="AF765" s="4"/>
       <c r="AG765" s="3"/>
     </row>
     <row r="766" spans="16:33" x14ac:dyDescent="0.3">
@@ -16938,9 +17281,9 @@
       <c r="AA766" s="5"/>
       <c r="AB766" s="4"/>
       <c r="AC766" s="4"/>
-      <c r="AD766" s="4"/>
-      <c r="AE766" s="4"/>
-      <c r="AF766" s="4"/>
+      <c r="AD766" s="3"/>
+      <c r="AE766" s="3"/>
+      <c r="AF766" s="3"/>
       <c r="AG766" s="3"/>
     </row>
     <row r="767" spans="16:33" x14ac:dyDescent="0.3">
@@ -18192,9 +18535,9 @@
       <c r="AA832" s="5"/>
       <c r="AB832" s="4"/>
       <c r="AC832" s="4"/>
-      <c r="AD832" s="3"/>
-      <c r="AE832" s="3"/>
-      <c r="AF832" s="3"/>
+      <c r="AD832" s="4"/>
+      <c r="AE832" s="4"/>
+      <c r="AF832" s="4"/>
       <c r="AG832" s="3"/>
     </row>
     <row r="833" spans="16:33" x14ac:dyDescent="0.3">
@@ -18231,8 +18574,8 @@
       <c r="AB834" s="4"/>
       <c r="AC834" s="4"/>
       <c r="AD834" s="4"/>
-      <c r="AE834" s="4"/>
-      <c r="AF834" s="4"/>
+      <c r="AE834" s="3"/>
+      <c r="AF834" s="3"/>
       <c r="AG834" s="3"/>
     </row>
     <row r="835" spans="16:33" x14ac:dyDescent="0.3">
@@ -18306,7 +18649,7 @@
       <c r="AA838" s="5"/>
       <c r="AB838" s="4"/>
       <c r="AC838" s="4"/>
-      <c r="AD838" s="4"/>
+      <c r="AD838" s="3"/>
       <c r="AE838" s="3"/>
       <c r="AF838" s="3"/>
       <c r="AG838" s="3"/>
@@ -18838,10 +19181,10 @@
       <c r="AA866" s="5"/>
       <c r="AB866" s="4"/>
       <c r="AC866" s="4"/>
-      <c r="AD866" s="3"/>
-      <c r="AE866" s="3"/>
-      <c r="AF866" s="3"/>
-      <c r="AG866" s="3"/>
+      <c r="AD866" s="4"/>
+      <c r="AE866" s="4"/>
+      <c r="AF866" s="4"/>
+      <c r="AG866" s="4"/>
     </row>
     <row r="867" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P867" s="4"/>
@@ -18879,7 +19222,7 @@
       <c r="AD868" s="4"/>
       <c r="AE868" s="4"/>
       <c r="AF868" s="4"/>
-      <c r="AG868" s="4"/>
+      <c r="AG868" s="3"/>
     </row>
     <row r="869" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P869" s="4"/>
@@ -18895,9 +19238,9 @@
       <c r="AA869" s="5"/>
       <c r="AB869" s="4"/>
       <c r="AC869" s="4"/>
-      <c r="AD869" s="4"/>
-      <c r="AE869" s="4"/>
-      <c r="AF869" s="4"/>
+      <c r="AD869" s="3"/>
+      <c r="AE869" s="3"/>
+      <c r="AF869" s="3"/>
       <c r="AG869" s="3"/>
     </row>
     <row r="870" spans="16:33" x14ac:dyDescent="0.3">
@@ -19579,10 +19922,10 @@
       <c r="AA905" s="5"/>
       <c r="AB905" s="4"/>
       <c r="AC905" s="4"/>
-      <c r="AD905" s="3"/>
-      <c r="AE905" s="3"/>
-      <c r="AF905" s="3"/>
-      <c r="AG905" s="3"/>
+      <c r="AD905" s="4"/>
+      <c r="AE905" s="4"/>
+      <c r="AF905" s="4"/>
+      <c r="AG905" s="4"/>
     </row>
     <row r="906" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P906" s="4"/>
@@ -19848,7 +20191,7 @@
       <c r="AD919" s="4"/>
       <c r="AE919" s="4"/>
       <c r="AF919" s="4"/>
-      <c r="AG919" s="4"/>
+      <c r="AG919" s="3"/>
     </row>
     <row r="920" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P920" s="4"/>
@@ -19867,7 +20210,7 @@
       <c r="AD920" s="4"/>
       <c r="AE920" s="4"/>
       <c r="AF920" s="4"/>
-      <c r="AG920" s="3"/>
+      <c r="AG920" s="4"/>
     </row>
     <row r="921" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P921" s="4"/>
@@ -19902,10 +20245,10 @@
       <c r="AA922" s="5"/>
       <c r="AB922" s="4"/>
       <c r="AC922" s="4"/>
-      <c r="AD922" s="4"/>
-      <c r="AE922" s="4"/>
-      <c r="AF922" s="4"/>
-      <c r="AG922" s="4"/>
+      <c r="AD922" s="3"/>
+      <c r="AE922" s="3"/>
+      <c r="AF922" s="3"/>
+      <c r="AG922" s="3"/>
     </row>
     <row r="923" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P923" s="4"/>
@@ -20320,10 +20663,10 @@
       <c r="AA944" s="5"/>
       <c r="AB944" s="4"/>
       <c r="AC944" s="4"/>
-      <c r="AD944" s="3"/>
-      <c r="AE944" s="3"/>
-      <c r="AF944" s="3"/>
-      <c r="AG944" s="3"/>
+      <c r="AD944" s="4"/>
+      <c r="AE944" s="4"/>
+      <c r="AF944" s="4"/>
+      <c r="AG944" s="4"/>
     </row>
     <row r="945" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P945" s="4"/>
@@ -20494,7 +20837,7 @@
       <c r="AD953" s="4"/>
       <c r="AE953" s="4"/>
       <c r="AF953" s="4"/>
-      <c r="AG953" s="4"/>
+      <c r="AG953" s="3"/>
     </row>
     <row r="954" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P954" s="4"/>
@@ -20510,9 +20853,9 @@
       <c r="AA954" s="5"/>
       <c r="AB954" s="4"/>
       <c r="AC954" s="4"/>
-      <c r="AD954" s="4"/>
-      <c r="AE954" s="4"/>
-      <c r="AF954" s="4"/>
+      <c r="AD954" s="3"/>
+      <c r="AE954" s="3"/>
+      <c r="AF954" s="3"/>
       <c r="AG954" s="3"/>
     </row>
     <row r="955" spans="16:33" x14ac:dyDescent="0.3">
@@ -20852,10 +21195,10 @@
       <c r="AA972" s="5"/>
       <c r="AB972" s="4"/>
       <c r="AC972" s="4"/>
-      <c r="AD972" s="3"/>
-      <c r="AE972" s="3"/>
-      <c r="AF972" s="3"/>
-      <c r="AG972" s="3"/>
+      <c r="AD972" s="4"/>
+      <c r="AE972" s="4"/>
+      <c r="AF972" s="4"/>
+      <c r="AG972" s="4"/>
     </row>
     <row r="973" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P973" s="4"/>
@@ -20947,10 +21290,10 @@
       <c r="AA977" s="5"/>
       <c r="AB977" s="4"/>
       <c r="AC977" s="4"/>
-      <c r="AD977" s="4"/>
-      <c r="AE977" s="4"/>
-      <c r="AF977" s="4"/>
-      <c r="AG977" s="4"/>
+      <c r="AD977" s="3"/>
+      <c r="AE977" s="3"/>
+      <c r="AF977" s="3"/>
+      <c r="AG977" s="3"/>
     </row>
     <row r="978" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P978" s="4"/>
@@ -22144,10 +22487,10 @@
       <c r="AA1040" s="5"/>
       <c r="AB1040" s="4"/>
       <c r="AC1040" s="4"/>
-      <c r="AD1040" s="3"/>
-      <c r="AE1040" s="3"/>
-      <c r="AF1040" s="3"/>
-      <c r="AG1040" s="3"/>
+      <c r="AD1040" s="4"/>
+      <c r="AE1040" s="4"/>
+      <c r="AF1040" s="4"/>
+      <c r="AG1040" s="4"/>
     </row>
     <row r="1041" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P1041" s="4"/>
@@ -22163,10 +22506,10 @@
       <c r="AA1041" s="5"/>
       <c r="AB1041" s="4"/>
       <c r="AC1041" s="4"/>
-      <c r="AD1041" s="4"/>
-      <c r="AE1041" s="4"/>
-      <c r="AF1041" s="4"/>
-      <c r="AG1041" s="4"/>
+      <c r="AD1041" s="3"/>
+      <c r="AE1041" s="3"/>
+      <c r="AF1041" s="3"/>
+      <c r="AG1041" s="3"/>
     </row>
     <row r="1042" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P1042" s="4"/>
@@ -22619,10 +22962,10 @@
       <c r="AA1065" s="5"/>
       <c r="AB1065" s="4"/>
       <c r="AC1065" s="4"/>
-      <c r="AD1065" s="3"/>
-      <c r="AE1065" s="3"/>
-      <c r="AF1065" s="3"/>
-      <c r="AG1065" s="3"/>
+      <c r="AD1065" s="4"/>
+      <c r="AE1065" s="4"/>
+      <c r="AF1065" s="4"/>
+      <c r="AG1065" s="4"/>
     </row>
     <row r="1066" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P1066" s="4"/>
@@ -22658,9 +23001,9 @@
       <c r="AB1067" s="4"/>
       <c r="AC1067" s="4"/>
       <c r="AD1067" s="4"/>
-      <c r="AE1067" s="4"/>
+      <c r="AE1067" s="3"/>
       <c r="AF1067" s="4"/>
-      <c r="AG1067" s="4"/>
+      <c r="AG1067" s="3"/>
     </row>
     <row r="1068" spans="16:33" x14ac:dyDescent="0.3">
       <c r="P1068" s="4"/>
@@ -22695,9 +23038,9 @@
       <c r="AA1069" s="5"/>
       <c r="AB1069" s="4"/>
       <c r="AC1069" s="4"/>
-      <c r="AD1069" s="4"/>
+      <c r="AD1069" s="3"/>
       <c r="AE1069" s="3"/>
-      <c r="AF1069" s="4"/>
+      <c r="AF1069" s="3"/>
       <c r="AG1069" s="3"/>
     </row>
     <row r="1070" spans="16:33" x14ac:dyDescent="0.3">
@@ -23099,29 +23442,11 @@
       <c r="AF1090" s="3"/>
       <c r="AG1090" s="3"/>
     </row>
-    <row r="1091" spans="16:33" x14ac:dyDescent="0.3">
-      <c r="P1091" s="4"/>
-      <c r="Q1091" s="4"/>
-      <c r="R1091" s="5"/>
-      <c r="T1091" s="5"/>
-      <c r="U1091" s="5"/>
-      <c r="V1091" s="5"/>
-      <c r="W1091" s="5"/>
-      <c r="X1091" s="5"/>
-      <c r="Y1091" s="5"/>
-      <c r="Z1091" s="5"/>
-      <c r="AA1091" s="5"/>
-      <c r="AB1091" s="4"/>
-      <c r="AC1091" s="4"/>
-      <c r="AD1091" s="3"/>
-      <c r="AE1091" s="3"/>
-      <c r="AF1091" s="3"/>
-      <c r="AG1091" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>